<commit_message>
all audio assets added
</commit_message>
<xml_diff>
--- a/Timeline/timeline.xlsx
+++ b/Timeline/timeline.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Hussnain\Desktop\AXWORLD-master\Timeline\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hussn\Desktop\AXWORLD\Timeline\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{9203A46A-DEFE-48AF-9007-48D36F874DDF}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7188DF0-D32A-4F23-A231-0F411F899C72}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{D94A9A97-B766-4125-AEC3-8A9ABAA42FC1}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D94A9A97-B766-4125-AEC3-8A9ABAA42FC1}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="44">
   <si>
     <t>Objectives</t>
   </si>
@@ -148,13 +148,28 @@
   </si>
   <si>
     <t>Choose topic</t>
+  </si>
+  <si>
+    <t>Glass Shatering</t>
+  </si>
+  <si>
+    <t>Walking Over Glass</t>
+  </si>
+  <si>
+    <t>Dumpster Sound</t>
+  </si>
+  <si>
+    <t>Falling Down</t>
+  </si>
+  <si>
+    <t>Broken UFO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -165,6 +180,13 @@
     <font>
       <sz val="11"/>
       <color rgb="FF00B0F0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF7030A0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -208,12 +230,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -528,10 +551,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{905AA3CC-7068-4915-ACB1-1DE84227CE48}">
-  <dimension ref="A1:M28"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L12" sqref="L12"/>
+      <selection activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -631,19 +654,19 @@
       <c r="A10" t="s">
         <v>30</v>
       </c>
-      <c r="I10" s="2"/>
+      <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>29</v>
       </c>
-      <c r="J11" s="2"/>
+      <c r="J11" s="3"/>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>28</v>
       </c>
-      <c r="K12" s="2"/>
+      <c r="K12" s="3"/>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
@@ -655,7 +678,7 @@
       <c r="A14" t="s">
         <v>26</v>
       </c>
-      <c r="K14" s="2"/>
+      <c r="K14" s="3"/>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
@@ -679,7 +702,7 @@
       <c r="A18" t="s">
         <v>22</v>
       </c>
-      <c r="L18" s="2"/>
+      <c r="L18" s="3"/>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A19" s="1" t="s">
@@ -690,48 +713,79 @@
       <c r="A20" t="s">
         <v>20</v>
       </c>
-      <c r="L20" s="2"/>
+      <c r="L20" s="3"/>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
-      <c r="L21" s="2"/>
+      <c r="L21" s="3"/>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>18</v>
       </c>
-      <c r="L22" s="2"/>
+      <c r="L22" s="3"/>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>17</v>
       </c>
-      <c r="I23" s="2"/>
+      <c r="I23" s="5"/>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>16</v>
       </c>
-      <c r="J24" s="2"/>
+      <c r="J24" s="5"/>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>39</v>
+      </c>
+      <c r="L25" s="5"/>
     </row>
     <row r="26" spans="1:12" x14ac:dyDescent="0.3">
-      <c r="A26" s="1" t="s">
-        <v>15</v>
-      </c>
+      <c r="A26" t="s">
+        <v>40</v>
+      </c>
+      <c r="L26" s="5"/>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>14</v>
-      </c>
-      <c r="B27" s="2"/>
+        <v>41</v>
+      </c>
+      <c r="L27" s="3"/>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
+        <v>42</v>
+      </c>
+      <c r="L28" s="3"/>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>43</v>
+      </c>
+      <c r="L29" s="3"/>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A30" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="L30" s="3"/>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>14</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
         <v>13</v>
       </c>
-      <c r="B28" s="3"/>
+      <c r="B32" s="5"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>